<commit_message>
Support a sheet parameter for an excel source
</commit_message>
<xml_diff>
--- a/spec/arc-furnace/resources/excel.xlsx
+++ b/spec/arc-furnace/resources/excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dspangenberger/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dspangenberger/cs/arc-furnace/spec/arc-furnace/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -48,6 +49,15 @@
   </si>
   <si>
     <t>ColC</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
   </si>
 </sst>
 </file>
@@ -365,7 +375,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,4 +419,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>